<commit_message>
initialized R code, added metadata files
</commit_message>
<xml_diff>
--- a/Single_cell_analysis/Metadata_Testa_Organoids_Bulk_E_MTAB_8337.xlsx
+++ b/Single_cell_analysis/Metadata_Testa_Organoids_Bulk_E_MTAB_8337.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/eugenio_graceffo_charite_de/Documents/Schuelke_Lab/EG15_RNA_Seq/E-MTAB-8325-8337_Testa_Organoids/Single_cell_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4F768B4-0959-8C42-B350-8162788CFE31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{F4F768B4-0959-8C42-B350-8162788CFE31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54FC4357-BCA4-4F40-915F-D6A8716DA422}"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="22100" windowWidth="28040" windowHeight="15800" xr2:uid="{A0A58857-E25A-414F-AC5E-36C938AF7FC1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="12680" xr2:uid="{A0A58857-E25A-414F-AC5E-36C938AF7FC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1272,8 +1272,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AU20" sqref="AU20"/>
+    <sheetView tabSelected="1" topLeftCell="AO20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AX34" sqref="AX34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2215,25 +2215,25 @@
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>181</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>109</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>183</v>
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>60</v>
@@ -2275,7 +2275,7 @@
         <v>68</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>181</v>
+        <v>108</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>71</v>
@@ -2347,25 +2347,25 @@
         <v>68</v>
       </c>
       <c r="AS6" s="1" t="s">
-        <v>184</v>
+        <v>112</v>
       </c>
       <c r="AT6" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>185</v>
+        <v>113</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>186</v>
+        <v>114</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>186</v>
+        <v>114</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>187</v>
+        <v>115</v>
       </c>
       <c r="AY6" s="1" t="s">
-        <v>188</v>
+        <v>116</v>
       </c>
       <c r="AZ6" s="1" t="s">
         <v>82</v>
@@ -2375,7 +2375,7 @@
       <c r="BC6" s="1"/>
       <c r="BD6" s="1"/>
       <c r="BE6" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="BF6" s="1" t="s">
         <v>94</v>
@@ -2387,31 +2387,31 @@
         <v>64</v>
       </c>
       <c r="BI6" s="1" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
       <c r="BJ6" s="2"/>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>181</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>182</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>183</v>
+        <v>110</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>60</v>
@@ -2453,7 +2453,7 @@
         <v>68</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>181</v>
+        <v>108</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>71</v>
@@ -2525,25 +2525,25 @@
         <v>68</v>
       </c>
       <c r="AS7" s="1" t="s">
-        <v>184</v>
+        <v>112</v>
       </c>
       <c r="AT7" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU7" s="1" t="s">
-        <v>185</v>
+        <v>113</v>
       </c>
       <c r="AV7" s="1" t="s">
-        <v>190</v>
+        <v>118</v>
       </c>
       <c r="AW7" s="1" t="s">
-        <v>190</v>
+        <v>118</v>
       </c>
       <c r="AX7" s="1" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
       <c r="AY7" s="1" t="s">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="AZ7" s="1" t="s">
         <v>82</v>
@@ -2553,7 +2553,7 @@
       <c r="BC7" s="1"/>
       <c r="BD7" s="1"/>
       <c r="BE7" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="BF7" s="1" t="s">
         <v>94</v>
@@ -2565,7 +2565,7 @@
         <v>64</v>
       </c>
       <c r="BI7" s="1" t="s">
-        <v>193</v>
+        <v>121</v>
       </c>
       <c r="BJ7" s="2"/>
     </row>
@@ -4572,16 +4572,16 @@
         <v>185</v>
       </c>
       <c r="AV18" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="AW18" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="AX18" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="AY18" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="AZ18" s="1" t="s">
         <v>82</v>
@@ -4603,7 +4603,7 @@
         <v>64</v>
       </c>
       <c r="BI18" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="BJ18" s="2"/>
     </row>
@@ -4750,16 +4750,16 @@
         <v>185</v>
       </c>
       <c r="AV19" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="AW19" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="AX19" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="AY19" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="AZ19" s="1" t="s">
         <v>82</v>
@@ -4781,31 +4781,31 @@
         <v>64</v>
       </c>
       <c r="BI19" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="BJ19" s="2"/>
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>60</v>
@@ -4847,7 +4847,7 @@
         <v>68</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>71</v>
@@ -4919,25 +4919,25 @@
         <v>68</v>
       </c>
       <c r="AS20" s="1" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="AT20" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU20" s="1" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="AV20" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="AW20" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="AX20" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="AY20" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="AZ20" s="1" t="s">
         <v>82</v>
@@ -4959,31 +4959,31 @@
         <v>64</v>
       </c>
       <c r="BI20" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="BJ20" s="2"/>
     </row>
     <row r="21" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E21" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>60</v>
@@ -5025,7 +5025,7 @@
         <v>68</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>71</v>
@@ -5097,25 +5097,25 @@
         <v>68</v>
       </c>
       <c r="AS21" s="1" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="AT21" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU21" s="1" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="AV21" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="AW21" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="AX21" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="AY21" s="1" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="AZ21" s="1" t="s">
         <v>82</v>
@@ -5137,7 +5137,7 @@
         <v>64</v>
       </c>
       <c r="BI21" s="1" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="BJ21" s="2"/>
     </row>
@@ -5284,16 +5284,16 @@
         <v>206</v>
       </c>
       <c r="AV22" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="AW22" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="AX22" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="AY22" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="AZ22" s="1" t="s">
         <v>82</v>
@@ -5315,7 +5315,7 @@
         <v>64</v>
       </c>
       <c r="BI22" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="BJ22" s="2"/>
     </row>
@@ -5462,16 +5462,16 @@
         <v>206</v>
       </c>
       <c r="AV23" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="AW23" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="AX23" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="AY23" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="AZ23" s="1" t="s">
         <v>82</v>
@@ -5493,25 +5493,25 @@
         <v>64</v>
       </c>
       <c r="BI23" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="BJ23" s="2"/>
     </row>
     <row r="24" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E24" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>58</v>
@@ -5559,7 +5559,7 @@
         <v>68</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="V24" s="1" t="s">
         <v>71</v>
@@ -5631,25 +5631,25 @@
         <v>68</v>
       </c>
       <c r="AS24" s="1" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="AT24" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU24" s="1" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="AV24" s="1" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="AW24" s="1" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="AX24" s="1" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="AY24" s="1" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="AZ24" s="1" t="s">
         <v>82</v>
@@ -5671,25 +5671,25 @@
         <v>64</v>
       </c>
       <c r="BI24" s="1" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="BJ24" s="2"/>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E25" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>58</v>
@@ -5737,7 +5737,7 @@
         <v>68</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="V25" s="1" t="s">
         <v>71</v>
@@ -5809,25 +5809,25 @@
         <v>68</v>
       </c>
       <c r="AS25" s="1" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="AT25" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU25" s="1" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="AV25" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="AW25" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="AX25" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="AY25" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="AZ25" s="1" t="s">
         <v>82</v>
@@ -5849,7 +5849,7 @@
         <v>64</v>
       </c>
       <c r="BI25" s="1" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="BJ25" s="2"/>
     </row>
@@ -5996,16 +5996,16 @@
         <v>227</v>
       </c>
       <c r="AV26" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="AW26" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="AX26" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="AY26" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="AZ26" s="1" t="s">
         <v>82</v>
@@ -6027,7 +6027,7 @@
         <v>64</v>
       </c>
       <c r="BI26" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="BJ26" s="2"/>
     </row>
@@ -6174,16 +6174,16 @@
         <v>227</v>
       </c>
       <c r="AV27" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="AW27" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="AX27" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="AY27" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="AZ27" s="1" t="s">
         <v>82</v>
@@ -6205,19 +6205,19 @@
         <v>64</v>
       </c>
       <c r="BI27" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="BJ27" s="2"/>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>108</v>
+        <v>223</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>109</v>
+        <v>224</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>225</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>57</v>
@@ -6271,7 +6271,7 @@
         <v>68</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>108</v>
+        <v>223</v>
       </c>
       <c r="V28" s="1" t="s">
         <v>71</v>
@@ -6343,25 +6343,25 @@
         <v>68</v>
       </c>
       <c r="AS28" s="1" t="s">
-        <v>112</v>
+        <v>226</v>
       </c>
       <c r="AT28" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU28" s="1" t="s">
-        <v>113</v>
+        <v>227</v>
       </c>
       <c r="AV28" s="1" t="s">
-        <v>114</v>
+        <v>236</v>
       </c>
       <c r="AW28" s="1" t="s">
-        <v>114</v>
+        <v>236</v>
       </c>
       <c r="AX28" s="1" t="s">
-        <v>115</v>
+        <v>237</v>
       </c>
       <c r="AY28" s="1" t="s">
-        <v>116</v>
+        <v>238</v>
       </c>
       <c r="AZ28" s="1" t="s">
         <v>82</v>
@@ -6371,7 +6371,7 @@
       <c r="BC28" s="1"/>
       <c r="BD28" s="1"/>
       <c r="BE28" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="BF28" s="1" t="s">
         <v>94</v>
@@ -6383,19 +6383,19 @@
         <v>64</v>
       </c>
       <c r="BI28" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="BJ28" s="2"/>
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>108</v>
+        <v>223</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>109</v>
+        <v>224</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>110</v>
+        <v>225</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>57</v>
@@ -6449,7 +6449,7 @@
         <v>68</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>108</v>
+        <v>223</v>
       </c>
       <c r="V29" s="1" t="s">
         <v>71</v>
@@ -6521,25 +6521,25 @@
         <v>68</v>
       </c>
       <c r="AS29" s="1" t="s">
-        <v>112</v>
+        <v>226</v>
       </c>
       <c r="AT29" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU29" s="1" t="s">
-        <v>113</v>
+        <v>227</v>
       </c>
       <c r="AV29" s="1" t="s">
-        <v>118</v>
+        <v>240</v>
       </c>
       <c r="AW29" s="1" t="s">
-        <v>118</v>
+        <v>240</v>
       </c>
       <c r="AX29" s="1" t="s">
-        <v>119</v>
+        <v>241</v>
       </c>
       <c r="AY29" s="1" t="s">
-        <v>120</v>
+        <v>242</v>
       </c>
       <c r="AZ29" s="1" t="s">
         <v>82</v>
@@ -6549,7 +6549,7 @@
       <c r="BC29" s="1"/>
       <c r="BD29" s="1"/>
       <c r="BE29" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="BF29" s="1" t="s">
         <v>94</v>
@@ -6561,7 +6561,7 @@
         <v>64</v>
       </c>
       <c r="BI29" s="1" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="BJ29" s="2"/>
     </row>
@@ -7641,7 +7641,7 @@
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:BJ35">
-      <sortCondition ref="BE1:BE35"/>
+      <sortCondition ref="AU1:AU35"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -7649,8 +7649,8 @@
     <hyperlink ref="BJ3" r:id="rId2" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229842" xr:uid="{64AFD047-084B-3B43-AEAE-D6DB0E5F62B0}"/>
     <hyperlink ref="BJ4" r:id="rId3" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229843" xr:uid="{42EF0A2E-0655-BC44-976A-93AB643F300A}"/>
     <hyperlink ref="BJ5" r:id="rId4" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229844" xr:uid="{5EFEFD15-5BAA-3146-BDAA-42D4795EEAF6}"/>
-    <hyperlink ref="BJ28" r:id="rId5" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229851" xr:uid="{233B49F1-8FDC-D84C-B8D2-264A69203503}"/>
-    <hyperlink ref="BJ29" r:id="rId6" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229852" xr:uid="{CFAE303E-CF94-FC40-9A05-02FD0CCC0938}"/>
+    <hyperlink ref="BJ6" r:id="rId5" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229851" xr:uid="{233B49F1-8FDC-D84C-B8D2-264A69203503}"/>
+    <hyperlink ref="BJ7" r:id="rId6" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229852" xr:uid="{CFAE303E-CF94-FC40-9A05-02FD0CCC0938}"/>
     <hyperlink ref="BJ8" r:id="rId7" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229845" xr:uid="{F1026E57-7D0B-C242-945C-38500AF9403E}"/>
     <hyperlink ref="BJ9" r:id="rId8" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229846" xr:uid="{8BCB98BF-8076-4642-8959-E910042091EE}"/>
     <hyperlink ref="BJ10" r:id="rId9" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229847" xr:uid="{A1A7C062-B86D-E944-BDED-2D5D592B663E}"/>
@@ -7661,18 +7661,18 @@
     <hyperlink ref="BJ15" r:id="rId14" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229838" xr:uid="{3750B4BD-4E9F-9C45-8A04-B4F5BA02B425}"/>
     <hyperlink ref="BJ16" r:id="rId15" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229839" xr:uid="{93290032-2D54-ED40-A79B-BFFB67D7C3B2}"/>
     <hyperlink ref="BJ17" r:id="rId16" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229840" xr:uid="{2EBC9448-F8D0-6F4F-A9CE-AB0793B303AC}"/>
-    <hyperlink ref="BJ6" r:id="rId17" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229853" xr:uid="{2B13620F-5C76-F84E-9C13-155EBBBF4845}"/>
-    <hyperlink ref="BJ7" r:id="rId18" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229854" xr:uid="{84D68165-0936-4345-B88F-AF4CF8D3CD84}"/>
-    <hyperlink ref="BJ18" r:id="rId19" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229855" xr:uid="{145509B1-4650-4B49-8DC6-50FCFD01F3E5}"/>
-    <hyperlink ref="BJ19" r:id="rId20" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229856" xr:uid="{D7946AAF-305F-D247-865A-1F5F9D988F87}"/>
-    <hyperlink ref="BJ20" r:id="rId21" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229857" xr:uid="{F7ECD246-60E1-AC4F-8353-BD6C8CF96C28}"/>
-    <hyperlink ref="BJ21" r:id="rId22" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229858" xr:uid="{754B2EB3-CBED-B041-B5B0-4A973890942A}"/>
-    <hyperlink ref="BJ22" r:id="rId23" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229859" xr:uid="{09713317-191F-B14C-8FE0-962C886A9F0D}"/>
-    <hyperlink ref="BJ23" r:id="rId24" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229860" xr:uid="{FB14DD3C-1327-1E41-9B49-0D358E4ACA4B}"/>
-    <hyperlink ref="BJ24" r:id="rId25" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229861" xr:uid="{91DD34E0-F447-1448-A84C-DD1D82552A96}"/>
-    <hyperlink ref="BJ25" r:id="rId26" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229862" xr:uid="{D3E9950F-FF98-F34C-93E3-DCBD3C51E51E}"/>
-    <hyperlink ref="BJ26" r:id="rId27" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229863" xr:uid="{F142DBE2-BA92-4C45-89EE-484AE049E021}"/>
-    <hyperlink ref="BJ27" r:id="rId28" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229864" xr:uid="{FA7916FD-F186-624F-B985-687DEABD3F48}"/>
+    <hyperlink ref="BJ18" r:id="rId17" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229853" xr:uid="{2B13620F-5C76-F84E-9C13-155EBBBF4845}"/>
+    <hyperlink ref="BJ19" r:id="rId18" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229854" xr:uid="{84D68165-0936-4345-B88F-AF4CF8D3CD84}"/>
+    <hyperlink ref="BJ20" r:id="rId19" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229855" xr:uid="{145509B1-4650-4B49-8DC6-50FCFD01F3E5}"/>
+    <hyperlink ref="BJ21" r:id="rId20" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229856" xr:uid="{D7946AAF-305F-D247-865A-1F5F9D988F87}"/>
+    <hyperlink ref="BJ22" r:id="rId21" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229857" xr:uid="{F7ECD246-60E1-AC4F-8353-BD6C8CF96C28}"/>
+    <hyperlink ref="BJ23" r:id="rId22" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229858" xr:uid="{754B2EB3-CBED-B041-B5B0-4A973890942A}"/>
+    <hyperlink ref="BJ24" r:id="rId23" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229859" xr:uid="{09713317-191F-B14C-8FE0-962C886A9F0D}"/>
+    <hyperlink ref="BJ25" r:id="rId24" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229860" xr:uid="{FB14DD3C-1327-1E41-9B49-0D358E4ACA4B}"/>
+    <hyperlink ref="BJ26" r:id="rId25" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229861" xr:uid="{91DD34E0-F447-1448-A84C-DD1D82552A96}"/>
+    <hyperlink ref="BJ27" r:id="rId26" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229862" xr:uid="{D3E9950F-FF98-F34C-93E3-DCBD3C51E51E}"/>
+    <hyperlink ref="BJ28" r:id="rId27" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229863" xr:uid="{F142DBE2-BA92-4C45-89EE-484AE049E021}"/>
+    <hyperlink ref="BJ29" r:id="rId28" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229864" xr:uid="{FA7916FD-F186-624F-B985-687DEABD3F48}"/>
     <hyperlink ref="BJ30" r:id="rId29" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229865" xr:uid="{BFFA86CA-1A70-8145-B150-1F4D4B986FD5}"/>
     <hyperlink ref="BJ31" r:id="rId30" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229866" xr:uid="{8CBE1EB7-6A1C-0141-81F6-F755DEC12F89}"/>
     <hyperlink ref="BJ32" r:id="rId31" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229867" xr:uid="{E5EC0D05-7FA3-DF43-9D78-94D95411D0E7}"/>

</xml_diff>

<commit_message>
Updated R code to include Filtering QC steps for each sample separately
</commit_message>
<xml_diff>
--- a/Single_cell_analysis/Metadata_Testa_Organoids_Bulk_E_MTAB_8337.xlsx
+++ b/Single_cell_analysis/Metadata_Testa_Organoids_Bulk_E_MTAB_8337.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/eugenio_graceffo_charite_de/Documents/Schuelke_Lab/EG15_RNA_Seq/E-MTAB-8325-8337_Testa_Organoids/Single_cell_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F4F768B4-0959-8C42-B350-8162788CFE31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54FC4357-BCA4-4F40-915F-D6A8716DA422}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{F4F768B4-0959-8C42-B350-8162788CFE31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E69E13E0-26AC-0C41-853F-0B3DCA3C23F5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="12680" xr2:uid="{A0A58857-E25A-414F-AC5E-36C938AF7FC1}"/>
+    <workbookView xWindow="5220" yWindow="19540" windowWidth="20480" windowHeight="12680" xr2:uid="{A0A58857-E25A-414F-AC5E-36C938AF7FC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1272,8 +1272,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AX34" sqref="AX34"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AV34" sqref="AV34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2215,25 +2215,25 @@
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>60</v>
@@ -2275,7 +2275,7 @@
         <v>68</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>71</v>
@@ -2347,25 +2347,25 @@
         <v>68</v>
       </c>
       <c r="AS6" s="1" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="AT6" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>113</v>
+        <v>185</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="AY6" s="1" t="s">
-        <v>116</v>
+        <v>188</v>
       </c>
       <c r="AZ6" s="1" t="s">
         <v>82</v>
@@ -2375,7 +2375,7 @@
       <c r="BC6" s="1"/>
       <c r="BD6" s="1"/>
       <c r="BE6" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="BF6" s="1" t="s">
         <v>94</v>
@@ -2387,31 +2387,31 @@
         <v>64</v>
       </c>
       <c r="BI6" s="1" t="s">
-        <v>117</v>
+        <v>189</v>
       </c>
       <c r="BJ6" s="2"/>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>60</v>
@@ -2453,7 +2453,7 @@
         <v>68</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>71</v>
@@ -2525,25 +2525,25 @@
         <v>68</v>
       </c>
       <c r="AS7" s="1" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="AT7" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU7" s="1" t="s">
-        <v>113</v>
+        <v>185</v>
       </c>
       <c r="AV7" s="1" t="s">
-        <v>118</v>
+        <v>190</v>
       </c>
       <c r="AW7" s="1" t="s">
-        <v>118</v>
+        <v>190</v>
       </c>
       <c r="AX7" s="1" t="s">
-        <v>119</v>
+        <v>191</v>
       </c>
       <c r="AY7" s="1" t="s">
-        <v>120</v>
+        <v>192</v>
       </c>
       <c r="AZ7" s="1" t="s">
         <v>82</v>
@@ -2553,7 +2553,7 @@
       <c r="BC7" s="1"/>
       <c r="BD7" s="1"/>
       <c r="BE7" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="BF7" s="1" t="s">
         <v>94</v>
@@ -2565,7 +2565,7 @@
         <v>64</v>
       </c>
       <c r="BI7" s="1" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
       <c r="BJ7" s="2"/>
     </row>
@@ -4572,16 +4572,16 @@
         <v>185</v>
       </c>
       <c r="AV18" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="AW18" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="AX18" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="AY18" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="AZ18" s="1" t="s">
         <v>82</v>
@@ -4603,7 +4603,7 @@
         <v>64</v>
       </c>
       <c r="BI18" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="BJ18" s="2"/>
     </row>
@@ -4750,16 +4750,16 @@
         <v>185</v>
       </c>
       <c r="AV19" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="AW19" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="AX19" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="AY19" s="1" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="AZ19" s="1" t="s">
         <v>82</v>
@@ -4781,31 +4781,31 @@
         <v>64</v>
       </c>
       <c r="BI19" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="BJ19" s="2"/>
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E20" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>60</v>
@@ -4847,7 +4847,7 @@
         <v>68</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>71</v>
@@ -4919,25 +4919,25 @@
         <v>68</v>
       </c>
       <c r="AS20" s="1" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="AT20" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU20" s="1" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="AV20" s="1" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="AW20" s="1" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="AX20" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="AY20" s="1" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="AZ20" s="1" t="s">
         <v>82</v>
@@ -4959,31 +4959,31 @@
         <v>64</v>
       </c>
       <c r="BI20" s="1" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="BJ20" s="2"/>
     </row>
     <row r="21" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E21" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>60</v>
@@ -5025,7 +5025,7 @@
         <v>68</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>71</v>
@@ -5097,25 +5097,25 @@
         <v>68</v>
       </c>
       <c r="AS21" s="1" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="AT21" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU21" s="1" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="AV21" s="1" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="AW21" s="1" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="AX21" s="1" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="AY21" s="1" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="AZ21" s="1" t="s">
         <v>82</v>
@@ -5137,7 +5137,7 @@
         <v>64</v>
       </c>
       <c r="BI21" s="1" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="BJ21" s="2"/>
     </row>
@@ -5284,16 +5284,16 @@
         <v>206</v>
       </c>
       <c r="AV22" s="1" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="AW22" s="1" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="AX22" s="1" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="AY22" s="1" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="AZ22" s="1" t="s">
         <v>82</v>
@@ -5315,7 +5315,7 @@
         <v>64</v>
       </c>
       <c r="BI22" s="1" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="BJ22" s="2"/>
     </row>
@@ -5462,16 +5462,16 @@
         <v>206</v>
       </c>
       <c r="AV23" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="AW23" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="AX23" s="1" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="AY23" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="AZ23" s="1" t="s">
         <v>82</v>
@@ -5493,25 +5493,25 @@
         <v>64</v>
       </c>
       <c r="BI23" s="1" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="BJ23" s="2"/>
     </row>
     <row r="24" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>58</v>
@@ -5559,7 +5559,7 @@
         <v>68</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="V24" s="1" t="s">
         <v>71</v>
@@ -5631,25 +5631,25 @@
         <v>68</v>
       </c>
       <c r="AS24" s="1" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="AT24" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU24" s="1" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="AV24" s="1" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="AW24" s="1" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="AX24" s="1" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="AY24" s="1" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="AZ24" s="1" t="s">
         <v>82</v>
@@ -5671,25 +5671,25 @@
         <v>64</v>
       </c>
       <c r="BI24" s="1" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="BJ24" s="2"/>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>58</v>
@@ -5737,7 +5737,7 @@
         <v>68</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="V25" s="1" t="s">
         <v>71</v>
@@ -5809,25 +5809,25 @@
         <v>68</v>
       </c>
       <c r="AS25" s="1" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="AT25" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU25" s="1" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="AV25" s="1" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="AW25" s="1" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="AX25" s="1" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="AY25" s="1" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="AZ25" s="1" t="s">
         <v>82</v>
@@ -5849,7 +5849,7 @@
         <v>64</v>
       </c>
       <c r="BI25" s="1" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="BJ25" s="2"/>
     </row>
@@ -5996,16 +5996,16 @@
         <v>227</v>
       </c>
       <c r="AV26" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="AW26" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="AX26" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="AY26" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="AZ26" s="1" t="s">
         <v>82</v>
@@ -6027,7 +6027,7 @@
         <v>64</v>
       </c>
       <c r="BI26" s="1" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BJ26" s="2"/>
     </row>
@@ -6174,16 +6174,16 @@
         <v>227</v>
       </c>
       <c r="AV27" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="AW27" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="AX27" s="1" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="AY27" s="1" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="AZ27" s="1" t="s">
         <v>82</v>
@@ -6205,19 +6205,19 @@
         <v>64</v>
       </c>
       <c r="BI27" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="BJ27" s="2"/>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>223</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>224</v>
+        <v>109</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>225</v>
+        <v>110</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>57</v>
@@ -6271,7 +6271,7 @@
         <v>68</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>223</v>
+        <v>108</v>
       </c>
       <c r="V28" s="1" t="s">
         <v>71</v>
@@ -6343,25 +6343,25 @@
         <v>68</v>
       </c>
       <c r="AS28" s="1" t="s">
-        <v>226</v>
+        <v>112</v>
       </c>
       <c r="AT28" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU28" s="1" t="s">
-        <v>227</v>
+        <v>113</v>
       </c>
       <c r="AV28" s="1" t="s">
-        <v>236</v>
+        <v>114</v>
       </c>
       <c r="AW28" s="1" t="s">
-        <v>236</v>
+        <v>114</v>
       </c>
       <c r="AX28" s="1" t="s">
-        <v>237</v>
+        <v>115</v>
       </c>
       <c r="AY28" s="1" t="s">
-        <v>238</v>
+        <v>116</v>
       </c>
       <c r="AZ28" s="1" t="s">
         <v>82</v>
@@ -6371,7 +6371,7 @@
       <c r="BC28" s="1"/>
       <c r="BD28" s="1"/>
       <c r="BE28" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="BF28" s="1" t="s">
         <v>94</v>
@@ -6383,19 +6383,19 @@
         <v>64</v>
       </c>
       <c r="BI28" s="1" t="s">
-        <v>239</v>
+        <v>117</v>
       </c>
       <c r="BJ28" s="2"/>
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>223</v>
+        <v>108</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>224</v>
+        <v>109</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>225</v>
+        <v>110</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>57</v>
@@ -6449,7 +6449,7 @@
         <v>68</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>223</v>
+        <v>108</v>
       </c>
       <c r="V29" s="1" t="s">
         <v>71</v>
@@ -6521,25 +6521,25 @@
         <v>68</v>
       </c>
       <c r="AS29" s="1" t="s">
-        <v>226</v>
+        <v>112</v>
       </c>
       <c r="AT29" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AU29" s="1" t="s">
-        <v>227</v>
+        <v>113</v>
       </c>
       <c r="AV29" s="1" t="s">
-        <v>240</v>
+        <v>118</v>
       </c>
       <c r="AW29" s="1" t="s">
-        <v>240</v>
+        <v>118</v>
       </c>
       <c r="AX29" s="1" t="s">
-        <v>241</v>
+        <v>119</v>
       </c>
       <c r="AY29" s="1" t="s">
-        <v>242</v>
+        <v>120</v>
       </c>
       <c r="AZ29" s="1" t="s">
         <v>82</v>
@@ -6549,7 +6549,7 @@
       <c r="BC29" s="1"/>
       <c r="BD29" s="1"/>
       <c r="BE29" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="BF29" s="1" t="s">
         <v>94</v>
@@ -6561,7 +6561,7 @@
         <v>64</v>
       </c>
       <c r="BI29" s="1" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="BJ29" s="2"/>
     </row>
@@ -7641,7 +7641,7 @@
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:BJ35">
-      <sortCondition ref="AU1:AU35"/>
+      <sortCondition ref="BE1:BE35"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -7649,8 +7649,8 @@
     <hyperlink ref="BJ3" r:id="rId2" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229842" xr:uid="{64AFD047-084B-3B43-AEAE-D6DB0E5F62B0}"/>
     <hyperlink ref="BJ4" r:id="rId3" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229843" xr:uid="{42EF0A2E-0655-BC44-976A-93AB643F300A}"/>
     <hyperlink ref="BJ5" r:id="rId4" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229844" xr:uid="{5EFEFD15-5BAA-3146-BDAA-42D4795EEAF6}"/>
-    <hyperlink ref="BJ6" r:id="rId5" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229851" xr:uid="{233B49F1-8FDC-D84C-B8D2-264A69203503}"/>
-    <hyperlink ref="BJ7" r:id="rId6" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229852" xr:uid="{CFAE303E-CF94-FC40-9A05-02FD0CCC0938}"/>
+    <hyperlink ref="BJ28" r:id="rId5" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229851" xr:uid="{233B49F1-8FDC-D84C-B8D2-264A69203503}"/>
+    <hyperlink ref="BJ29" r:id="rId6" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229852" xr:uid="{CFAE303E-CF94-FC40-9A05-02FD0CCC0938}"/>
     <hyperlink ref="BJ8" r:id="rId7" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229845" xr:uid="{F1026E57-7D0B-C242-945C-38500AF9403E}"/>
     <hyperlink ref="BJ9" r:id="rId8" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229846" xr:uid="{8BCB98BF-8076-4642-8959-E910042091EE}"/>
     <hyperlink ref="BJ10" r:id="rId9" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229847" xr:uid="{A1A7C062-B86D-E944-BDED-2D5D592B663E}"/>
@@ -7661,18 +7661,18 @@
     <hyperlink ref="BJ15" r:id="rId14" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229838" xr:uid="{3750B4BD-4E9F-9C45-8A04-B4F5BA02B425}"/>
     <hyperlink ref="BJ16" r:id="rId15" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229839" xr:uid="{93290032-2D54-ED40-A79B-BFFB67D7C3B2}"/>
     <hyperlink ref="BJ17" r:id="rId16" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229840" xr:uid="{2EBC9448-F8D0-6F4F-A9CE-AB0793B303AC}"/>
-    <hyperlink ref="BJ18" r:id="rId17" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229853" xr:uid="{2B13620F-5C76-F84E-9C13-155EBBBF4845}"/>
-    <hyperlink ref="BJ19" r:id="rId18" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229854" xr:uid="{84D68165-0936-4345-B88F-AF4CF8D3CD84}"/>
-    <hyperlink ref="BJ20" r:id="rId19" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229855" xr:uid="{145509B1-4650-4B49-8DC6-50FCFD01F3E5}"/>
-    <hyperlink ref="BJ21" r:id="rId20" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229856" xr:uid="{D7946AAF-305F-D247-865A-1F5F9D988F87}"/>
-    <hyperlink ref="BJ22" r:id="rId21" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229857" xr:uid="{F7ECD246-60E1-AC4F-8353-BD6C8CF96C28}"/>
-    <hyperlink ref="BJ23" r:id="rId22" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229858" xr:uid="{754B2EB3-CBED-B041-B5B0-4A973890942A}"/>
-    <hyperlink ref="BJ24" r:id="rId23" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229859" xr:uid="{09713317-191F-B14C-8FE0-962C886A9F0D}"/>
-    <hyperlink ref="BJ25" r:id="rId24" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229860" xr:uid="{FB14DD3C-1327-1E41-9B49-0D358E4ACA4B}"/>
-    <hyperlink ref="BJ26" r:id="rId25" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229861" xr:uid="{91DD34E0-F447-1448-A84C-DD1D82552A96}"/>
-    <hyperlink ref="BJ27" r:id="rId26" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229862" xr:uid="{D3E9950F-FF98-F34C-93E3-DCBD3C51E51E}"/>
-    <hyperlink ref="BJ28" r:id="rId27" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229863" xr:uid="{F142DBE2-BA92-4C45-89EE-484AE049E021}"/>
-    <hyperlink ref="BJ29" r:id="rId28" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229864" xr:uid="{FA7916FD-F186-624F-B985-687DEABD3F48}"/>
+    <hyperlink ref="BJ6" r:id="rId17" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229853" xr:uid="{2B13620F-5C76-F84E-9C13-155EBBBF4845}"/>
+    <hyperlink ref="BJ7" r:id="rId18" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229854" xr:uid="{84D68165-0936-4345-B88F-AF4CF8D3CD84}"/>
+    <hyperlink ref="BJ18" r:id="rId19" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229855" xr:uid="{145509B1-4650-4B49-8DC6-50FCFD01F3E5}"/>
+    <hyperlink ref="BJ19" r:id="rId20" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229856" xr:uid="{D7946AAF-305F-D247-865A-1F5F9D988F87}"/>
+    <hyperlink ref="BJ20" r:id="rId21" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229857" xr:uid="{F7ECD246-60E1-AC4F-8353-BD6C8CF96C28}"/>
+    <hyperlink ref="BJ21" r:id="rId22" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229858" xr:uid="{754B2EB3-CBED-B041-B5B0-4A973890942A}"/>
+    <hyperlink ref="BJ22" r:id="rId23" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229859" xr:uid="{09713317-191F-B14C-8FE0-962C886A9F0D}"/>
+    <hyperlink ref="BJ23" r:id="rId24" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229860" xr:uid="{FB14DD3C-1327-1E41-9B49-0D358E4ACA4B}"/>
+    <hyperlink ref="BJ24" r:id="rId25" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229861" xr:uid="{91DD34E0-F447-1448-A84C-DD1D82552A96}"/>
+    <hyperlink ref="BJ25" r:id="rId26" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229862" xr:uid="{D3E9950F-FF98-F34C-93E3-DCBD3C51E51E}"/>
+    <hyperlink ref="BJ26" r:id="rId27" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229863" xr:uid="{F142DBE2-BA92-4C45-89EE-484AE049E021}"/>
+    <hyperlink ref="BJ27" r:id="rId28" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229864" xr:uid="{FA7916FD-F186-624F-B985-687DEABD3F48}"/>
     <hyperlink ref="BJ30" r:id="rId29" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229865" xr:uid="{BFFA86CA-1A70-8145-B150-1F4D4B986FD5}"/>
     <hyperlink ref="BJ31" r:id="rId30" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229866" xr:uid="{8CBE1EB7-6A1C-0141-81F6-F755DEC12F89}"/>
     <hyperlink ref="BJ32" r:id="rId31" display="https://www.ebi.ac.uk/ena/browser/view/ERR4229867" xr:uid="{E5EC0D05-7FA3-DF43-9D78-94D95411D0E7}"/>

</xml_diff>